<commit_message>
Changed base code to fix a bug (didn't show logs and other errors) Added Module for colissiones Started working on a JSON parser Aded an Excel file to store temporary the sizes of frames of the characters
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuelmb3\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Master\Programacion\Final Fight\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Cody" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Animación</t>
   </si>
@@ -49,11 +49,26 @@
   <si>
     <t>Caminar</t>
   </si>
+  <si>
+    <t>Saltar avanzando</t>
+  </si>
+  <si>
+    <t>Saltar estatico</t>
+  </si>
+  <si>
+    <t>Puñetazo simple</t>
+  </si>
+  <si>
+    <t>Puñetazo fuerte</t>
+  </si>
+  <si>
+    <t>Gancho</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,6 +116,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +429,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
@@ -433,7 +451,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
@@ -450,12 +468,12 @@
         <v>46</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F14" si="0">84-D3</f>
+        <f t="shared" ref="F3" si="0">84-D3</f>
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
@@ -476,7 +494,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5">
         <f t="shared" ref="B5:B14" si="1">B4+1</f>
         <v>3</v>
@@ -497,7 +515,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -518,7 +536,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -539,7 +557,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -560,7 +578,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -581,7 +599,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -602,7 +620,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -623,7 +641,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -644,7 +662,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -665,7 +683,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -685,9 +703,496 @@
         <v>91</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>186</v>
+      </c>
+      <c r="E15">
+        <f>85-C15</f>
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <f>268-D15</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16">
+        <f>1+B15</f>
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>125</v>
+      </c>
+      <c r="D16">
+        <v>156</v>
+      </c>
+      <c r="E16">
+        <f>166-C16</f>
+        <v>41</v>
+      </c>
+      <c r="F16">
+        <f>263-D16</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17">
+        <f t="shared" ref="B17:B23" si="2">1+B16</f>
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>199</v>
+      </c>
+      <c r="D17">
+        <v>156</v>
+      </c>
+      <c r="E17">
+        <f>253-C17</f>
+        <v>54</v>
+      </c>
+      <c r="F17">
+        <f>232-D17</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>283</v>
+      </c>
+      <c r="D18">
+        <v>159</v>
+      </c>
+      <c r="E18">
+        <f>352-C18</f>
+        <v>69</v>
+      </c>
+      <c r="F18">
+        <f>244-D18</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>377</v>
+      </c>
+      <c r="D19">
+        <v>171</v>
+      </c>
+      <c r="E19">
+        <f>458-C19</f>
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <f>223-D19</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>488</v>
+      </c>
+      <c r="D20">
+        <v>161</v>
+      </c>
+      <c r="E20">
+        <f>552-C20</f>
+        <v>64</v>
+      </c>
+      <c r="F20">
+        <f>221-D20</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>582</v>
+      </c>
+      <c r="D21">
+        <v>167</v>
+      </c>
+      <c r="E21">
+        <f>663-C21</f>
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <f>219-D21</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>697</v>
+      </c>
+      <c r="D22">
+        <v>167</v>
+      </c>
+      <c r="E22">
+        <f>761-C22</f>
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <f>227-D22</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>186</v>
+      </c>
+      <c r="E23">
+        <f>85-C23</f>
+        <v>53</v>
+      </c>
+      <c r="F23">
+        <f>268-D23</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>186</v>
+      </c>
+      <c r="E24">
+        <f>85-C24</f>
+        <v>53</v>
+      </c>
+      <c r="F24">
+        <f>268-D24</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25">
+        <f>1+B24</f>
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>125</v>
+      </c>
+      <c r="D25">
+        <v>156</v>
+      </c>
+      <c r="E25">
+        <f>166-C25</f>
+        <v>41</v>
+      </c>
+      <c r="F25">
+        <f>263-D25</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26">
+        <f t="shared" ref="B26:B28" si="3">1+B25</f>
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>199</v>
+      </c>
+      <c r="D26">
+        <v>156</v>
+      </c>
+      <c r="E26">
+        <f>253-C26</f>
+        <v>54</v>
+      </c>
+      <c r="F26">
+        <f>232-D26</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>283</v>
+      </c>
+      <c r="D27">
+        <v>159</v>
+      </c>
+      <c r="E27">
+        <f>352-C27</f>
+        <v>69</v>
+      </c>
+      <c r="F27">
+        <f>244-D27</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>32</v>
+      </c>
+      <c r="D28">
+        <v>186</v>
+      </c>
+      <c r="E28">
+        <f>85-C28</f>
+        <v>53</v>
+      </c>
+      <c r="F28">
+        <f>268-D28</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>316</v>
+      </c>
+      <c r="E29">
+        <f>92-C29</f>
+        <v>63</v>
+      </c>
+      <c r="F29">
+        <f>405-D29</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>127</v>
+      </c>
+      <c r="D30">
+        <v>313</v>
+      </c>
+      <c r="E30">
+        <f>210-C30</f>
+        <v>83</v>
+      </c>
+      <c r="F30">
+        <f>402-D30</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>237</v>
+      </c>
+      <c r="D31">
+        <v>321</v>
+      </c>
+      <c r="E31">
+        <f>304-C31</f>
+        <v>67</v>
+      </c>
+      <c r="F31">
+        <f>401-D31</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>333</v>
+      </c>
+      <c r="D32">
+        <v>324</v>
+      </c>
+      <c r="E32">
+        <f>442-C32</f>
+        <v>109</v>
+      </c>
+      <c r="F32">
+        <f>401-D32</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>465</v>
+      </c>
+      <c r="D33">
+        <v>320</v>
+      </c>
+      <c r="E33">
+        <f>532-C33</f>
+        <v>67</v>
+      </c>
+      <c r="F33">
+        <f>400-D33</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>559</v>
+      </c>
+      <c r="D34">
+        <v>334</v>
+      </c>
+      <c r="E34">
+        <f>637-C34</f>
+        <v>78</v>
+      </c>
+      <c r="F34">
+        <f>403-D34</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>668</v>
+      </c>
+      <c r="D35">
+        <v>325</v>
+      </c>
+      <c r="E35">
+        <f>750-C35</f>
+        <v>82</v>
+      </c>
+      <c r="F35">
+        <f>402-D35</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>774</v>
+      </c>
+      <c r="D36">
+        <v>315</v>
+      </c>
+      <c r="E36">
+        <f>853-C36</f>
+        <v>79</v>
+      </c>
+      <c r="F36">
+        <f>405-D36</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>874</v>
+      </c>
+      <c r="D37">
+        <v>293</v>
+      </c>
+      <c r="E37">
+        <f>929-C37</f>
+        <v>55</v>
+      </c>
+      <c r="F37">
+        <f>403-D37</f>
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
     <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Jump and Jump Forward animations for player done
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -106,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -120,6 +120,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,12 +443,10 @@
         <v>25</v>
       </c>
       <c r="E2">
-        <f>117-C2</f>
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <f>84-D2</f>
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -468,8 +467,7 @@
         <v>46</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3" si="0">84-D3</f>
-        <v>58</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -489,14 +487,13 @@
         <v>61</v>
       </c>
       <c r="F4">
-        <f>118-D4</f>
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5">
-        <f t="shared" ref="B5:B14" si="1">B4+1</f>
+        <f t="shared" ref="B5:B14" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5">
@@ -510,14 +507,13 @@
         <v>61</v>
       </c>
       <c r="F5">
-        <f>121-D5</f>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6">
@@ -531,14 +527,13 @@
         <v>48</v>
       </c>
       <c r="F6">
-        <f>123-D6</f>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C7">
@@ -552,14 +547,13 @@
         <v>30</v>
       </c>
       <c r="F7">
-        <f>121-D7</f>
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8">
@@ -573,14 +567,13 @@
         <v>29</v>
       </c>
       <c r="F8">
-        <f>121-D8</f>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C9">
@@ -594,14 +587,13 @@
         <v>46</v>
       </c>
       <c r="F9">
-        <f>119-D9</f>
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10">
@@ -615,14 +607,13 @@
         <v>61</v>
       </c>
       <c r="F10">
-        <f>120-D10</f>
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C11">
@@ -636,14 +627,13 @@
         <v>60</v>
       </c>
       <c r="F11">
-        <f>122-D11</f>
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C12">
@@ -657,14 +647,13 @@
         <v>50</v>
       </c>
       <c r="F12">
-        <f>122-D12</f>
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C13">
@@ -685,7 +674,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C14">
@@ -699,8 +688,7 @@
         <v>31</v>
       </c>
       <c r="F14">
-        <f>119-D14</f>
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +737,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17">
-        <f t="shared" ref="B17:B23" si="2">1+B16</f>
+        <f t="shared" ref="B17:B23" si="1">1+B16</f>
         <v>3</v>
       </c>
       <c r="C17">
@@ -770,7 +758,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C18">
@@ -791,7 +779,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C19">
@@ -812,7 +800,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C20">
@@ -833,7 +821,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C21">
@@ -854,7 +842,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C22">
@@ -875,7 +863,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C23">
@@ -939,7 +927,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26">
-        <f t="shared" ref="B26:B28" si="3">1+B25</f>
+        <f t="shared" ref="B26:B28" si="2">1+B25</f>
         <v>3</v>
       </c>
       <c r="C26">
@@ -960,7 +948,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C27">
@@ -981,7 +969,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C28">
@@ -1017,8 +1005,7 @@
         <v>63</v>
       </c>
       <c r="F29">
-        <f>405-D29</f>
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1037,8 +1024,7 @@
         <v>83</v>
       </c>
       <c r="F30">
-        <f>402-D30</f>
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,9 +1044,8 @@
         <f>304-C31</f>
         <v>67</v>
       </c>
-      <c r="F31">
-        <f>401-D31</f>
-        <v>80</v>
+      <c r="F31" s="5">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,12 +1060,10 @@
         <v>324</v>
       </c>
       <c r="E32">
-        <f>442-C32</f>
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F32">
-        <f>401-D32</f>
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,8 +1084,7 @@
         <v>67</v>
       </c>
       <c r="F33">
-        <f>400-D33</f>
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1121,8 +1103,7 @@
         <v>78</v>
       </c>
       <c r="F34">
-        <f>403-D34</f>
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1141,8 +1122,7 @@
         <v>82</v>
       </c>
       <c r="F35">
-        <f>402-D35</f>
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,8 +1141,7 @@
         <v>79</v>
       </c>
       <c r="F36">
-        <f>405-D36</f>
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1181,8 +1160,7 @@
         <v>55</v>
       </c>
       <c r="F37">
-        <f>403-D37</f>
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Player animations added: receive hit, fall, try to get up and get up
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Animación</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Gancho</t>
+  </si>
+  <si>
+    <t>Recibir daño</t>
+  </si>
+  <si>
+    <t>Caerse</t>
+  </si>
+  <si>
+    <t>Intentar levantarse</t>
+  </si>
+  <si>
+    <t>Levantarse</t>
   </si>
 </sst>
 </file>
@@ -106,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,13 +126,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +463,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3">
@@ -471,7 +484,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4">
         <f>B3+1</f>
         <v>2</v>
@@ -491,7 +504,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5">
         <f t="shared" ref="B5:B14" si="0">B4+1</f>
         <v>3</v>
@@ -511,7 +524,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -531,7 +544,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -551,7 +564,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -571,7 +584,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -591,7 +604,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -611,7 +624,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -631,7 +644,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -651,7 +664,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -672,7 +685,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -692,7 +705,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15">
@@ -714,7 +727,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16">
         <f>1+B15</f>
         <v>2</v>
@@ -735,7 +748,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17">
         <f t="shared" ref="B17:B23" si="1">1+B16</f>
         <v>3</v>
@@ -756,7 +769,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -777,7 +790,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="B19">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -798,7 +811,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -819,7 +832,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="B21">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -840,7 +853,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -861,7 +874,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="B23">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -882,7 +895,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B24">
@@ -904,7 +917,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
       <c r="B25">
         <f>1+B24</f>
         <v>2</v>
@@ -925,7 +938,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="B26">
         <f t="shared" ref="B26:B28" si="2">1+B25</f>
         <v>3</v>
@@ -946,7 +959,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="B27">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -967,7 +980,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -988,7 +1001,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B29">
@@ -1009,7 +1022,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30">
         <v>2</v>
       </c>
@@ -1028,7 +1041,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B31">
@@ -1044,12 +1057,12 @@
         <f>304-C31</f>
         <v>67</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="3">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32">
         <v>2</v>
       </c>
@@ -1067,7 +1080,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B33">
@@ -1088,7 +1101,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="B34">
         <v>2</v>
       </c>
@@ -1107,7 +1120,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="5"/>
       <c r="B35">
         <v>3</v>
       </c>
@@ -1126,7 +1139,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="B36">
         <v>4</v>
       </c>
@@ -1145,7 +1158,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="5"/>
       <c r="B37">
         <v>5</v>
       </c>
@@ -1163,8 +1176,214 @@
         <v>111</v>
       </c>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>26</v>
+      </c>
+      <c r="D38">
+        <v>712</v>
+      </c>
+      <c r="E38">
+        <f>80-C38</f>
+        <v>54</v>
+      </c>
+      <c r="F38">
+        <f>795-D38</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>112</v>
+      </c>
+      <c r="D39">
+        <v>700</v>
+      </c>
+      <c r="E39">
+        <f>172-C39</f>
+        <v>60</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39:F47" si="3">795-D39</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>214</v>
+      </c>
+      <c r="D40">
+        <v>704</v>
+      </c>
+      <c r="E40">
+        <f>308-C40</f>
+        <v>94</v>
+      </c>
+      <c r="F40">
+        <f>756-D40</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>337</v>
+      </c>
+      <c r="D41">
+        <v>753</v>
+      </c>
+      <c r="E41">
+        <f>453-C41</f>
+        <v>116</v>
+      </c>
+      <c r="F41">
+        <f>789-D41</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>337</v>
+      </c>
+      <c r="D42">
+        <v>753</v>
+      </c>
+      <c r="E42">
+        <f>453-C42</f>
+        <v>116</v>
+      </c>
+      <c r="F42">
+        <f>789-D42</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>481</v>
+      </c>
+      <c r="D43">
+        <v>759</v>
+      </c>
+      <c r="E43">
+        <f>574-C43</f>
+        <v>93</v>
+      </c>
+      <c r="F43">
+        <f>793-D43</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>337</v>
+      </c>
+      <c r="D44">
+        <v>753</v>
+      </c>
+      <c r="E44">
+        <f>453-C44</f>
+        <v>116</v>
+      </c>
+      <c r="F44">
+        <f>789-D44</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>481</v>
+      </c>
+      <c r="D45">
+        <v>759</v>
+      </c>
+      <c r="E45">
+        <f>574-C45</f>
+        <v>93</v>
+      </c>
+      <c r="F45">
+        <f>793-D45</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>602</v>
+      </c>
+      <c r="D46">
+        <v>739</v>
+      </c>
+      <c r="E46">
+        <f>655-C46</f>
+        <v>53</v>
+      </c>
+      <c r="F46">
+        <f>797-D46</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>31</v>
+      </c>
+      <c r="D47">
+        <v>25</v>
+      </c>
+      <c r="E47">
+        <v>59</v>
+      </c>
+      <c r="F47">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A47"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A28"/>

</xml_diff>

<commit_message>
Added Enemy and improve github page
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,7 +133,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1176,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B38">
@@ -1194,76 +1193,72 @@
         <v>54</v>
       </c>
       <c r="F38">
-        <f>795-D38</f>
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5"/>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3">
+        <v>31</v>
+      </c>
+      <c r="D39" s="3">
+        <v>25</v>
+      </c>
+      <c r="E39" s="3">
+        <v>59</v>
+      </c>
+      <c r="F39" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>112</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>700</v>
       </c>
-      <c r="E39">
-        <f>172-C39</f>
+      <c r="E40">
+        <f>172-C40</f>
         <v>60</v>
       </c>
-      <c r="F39">
-        <f t="shared" ref="F39:F47" si="3">795-D39</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="F40">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41">
         <v>2</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>214</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <v>704</v>
       </c>
-      <c r="E40">
-        <f>308-C40</f>
+      <c r="E41">
+        <f>308-C41</f>
         <v>94</v>
       </c>
-      <c r="F40">
-        <f>756-D40</f>
+      <c r="F41" s="3">
+        <f>756-D41</f>
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42">
         <v>3</v>
-      </c>
-      <c r="C41">
-        <v>337</v>
-      </c>
-      <c r="D41">
-        <v>753</v>
-      </c>
-      <c r="E41">
-        <f>453-C41</f>
-        <v>116</v>
-      </c>
-      <c r="F41">
-        <f>789-D41</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
       </c>
       <c r="C42">
         <v>337</v>
@@ -1280,110 +1275,133 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>337</v>
+      </c>
+      <c r="D43">
+        <v>753</v>
+      </c>
+      <c r="E43">
+        <f>453-C43</f>
+        <v>116</v>
+      </c>
+      <c r="F43">
+        <f>789-D43</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44">
         <v>2</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>481</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>759</v>
       </c>
-      <c r="E43">
-        <f>574-C43</f>
+      <c r="E44">
+        <f>574-C44</f>
         <v>93</v>
       </c>
-      <c r="F43">
-        <f>793-D43</f>
+      <c r="F44">
+        <f>793-D44</f>
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>1</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>337</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>753</v>
       </c>
-      <c r="E44">
-        <f>453-C44</f>
+      <c r="E45">
+        <f>453-C45</f>
         <v>116</v>
       </c>
-      <c r="F44">
-        <f>789-D44</f>
+      <c r="F45">
+        <f>789-D45</f>
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>481</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>759</v>
       </c>
-      <c r="E45">
-        <f>574-C45</f>
+      <c r="E46">
+        <f>574-C46</f>
         <v>93</v>
       </c>
-      <c r="F45">
-        <f>793-D45</f>
+      <c r="F46">
+        <f>793-D46</f>
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47">
         <v>3</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>602</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>739</v>
       </c>
-      <c r="E46">
-        <f>655-C46</f>
+      <c r="E47">
+        <f>655-C47</f>
         <v>53</v>
       </c>
-      <c r="F46">
-        <f>797-D46</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47">
+      <c r="F47">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48">
         <v>4</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>31</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>25</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <v>59</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A47"/>
+  <mergeCells count="10">
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A48"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A24:A28"/>

</xml_diff>